<commit_message>
evaluations for min/max width tolerance
max shows greatest improvement
</commit_message>
<xml_diff>
--- a/P-R_meanDetectionScore_9SP_chart.xlsx
+++ b/P-R_meanDetectionScore_9SP_chart.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="P-R_meanDetectionScore_9SP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -685,11 +685,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82731392"/>
-        <c:axId val="82709120"/>
+        <c:axId val="98349824"/>
+        <c:axId val="98351360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82731392"/>
+        <c:axId val="98349824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -697,12 +697,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82709120"/>
+        <c:crossAx val="98351360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82709120"/>
+        <c:axId val="98351360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -711,7 +711,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82731392"/>
+        <c:crossAx val="98349824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -724,7 +724,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -735,15 +735,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>